<commit_message>
Updates to EMEP inventory scaling 1. Remove scaling to blr. This is already scaled in EDGARv4.3.2 and scaling again here results in values that are too large in the historical timeseries. 2. Add scaling to BC in NFR14 3. Update EMEP NFR14 inventory data 4. Include an offical sector mapping table for EMEP emissions 5. Update the mapping files to correct for previous issues.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_NFR09_scaling_mapping.xlsx
+++ b/input/mappings/scaling/EMEP_NFR09_scaling_mapping.xlsx
@@ -1,18 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487C62C6-C539-F747-9774-590FB3F47368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="method" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="102">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -221,9 +233,6 @@
     <t>AgriLivestock</t>
   </si>
   <si>
-    <t>AgriOther</t>
-  </si>
-  <si>
     <t>2D3_Chemical-products-manufacture-processing</t>
   </si>
   <si>
@@ -321,12 +330,21 @@
   </si>
   <si>
     <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>EMEP data includes crop burning (so don’t scale)</t>
+  </si>
+  <si>
+    <t>blr</t>
+  </si>
+  <si>
+    <t>don’t scale before 2007 since this time period was already scaled to EDGAR and SF's will change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -922,6 +940,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1248,14 +1269,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
@@ -1263,7 +1284,7 @@
     <col min="5" max="6" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1276,7 +1297,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1289,7 +1310,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -1299,7 +1320,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -1309,9 +1330,9 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -1322,7 +1343,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>55</v>
       </c>
@@ -1332,7 +1353,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -1342,7 +1363,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>55</v>
       </c>
@@ -1352,7 +1373,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>55</v>
       </c>
@@ -1362,7 +1383,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>55</v>
       </c>
@@ -1372,7 +1393,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>55</v>
       </c>
@@ -1382,7 +1403,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -1392,7 +1413,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>55</v>
       </c>
@@ -1402,7 +1423,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>55</v>
       </c>
@@ -1412,7 +1433,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>55</v>
       </c>
@@ -1422,7 +1443,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>55</v>
       </c>
@@ -1432,7 +1453,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>55</v>
       </c>
@@ -1441,7 +1462,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>55</v>
       </c>
@@ -1450,9 +1471,9 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
         <v>57</v>
@@ -1462,7 +1483,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>57</v>
       </c>
@@ -1470,7 +1491,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>57</v>
       </c>
@@ -1478,92 +1499,92 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
         <v>31</v>
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
         <v>33</v>
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
         <v>36</v>
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
         <v>36</v>
       </c>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
         <v>58</v>
@@ -1573,7 +1594,7 @@
       </c>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>58</v>
       </c>
@@ -1582,7 +1603,7 @@
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>58</v>
       </c>
@@ -1591,7 +1612,7 @@
       </c>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>58</v>
       </c>
@@ -1600,16 +1621,16 @@
       </c>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>58</v>
       </c>
@@ -1618,21 +1639,21 @@
       </c>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
         <v>22</v>
@@ -1640,46 +1661,46 @@
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
         <v>63</v>
@@ -1691,7 +1712,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>63</v>
       </c>
@@ -1702,7 +1723,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>63</v>
       </c>
@@ -1713,17 +1734,17 @@
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D46" s="2"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
         <v>39</v>
@@ -1732,9 +1753,9 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
         <v>40</v>
@@ -1743,12 +1764,12 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C49" t="s">
         <v>41</v>
@@ -1757,12 +1778,12 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
         <v>42</v>
@@ -1770,15 +1791,15 @@
       <c r="E50" s="1"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E51" s="1"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E52" s="1"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -1791,7 +1812,7 @@
       <c r="E53" s="1"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
         <v>65</v>
       </c>
@@ -1801,331 +1822,325 @@
       <c r="E54" s="1"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="E55" s="1"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>47</v>
       </c>
-      <c r="B56" t="s">
-        <v>66</v>
-      </c>
       <c r="C56" t="s">
         <v>38</v>
       </c>
+      <c r="E56" t="s">
+        <v>99</v>
+      </c>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
-      <c r="B57" t="s">
-        <v>66</v>
-      </c>
       <c r="C57" t="s">
         <v>60</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
-      <c r="B58" t="s">
-        <v>66</v>
-      </c>
       <c r="C58" t="s">
         <v>61</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
         <v>43</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C65" s="4"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="C75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="C76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="C77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="C78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="C79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="1"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="1"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="1"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E94" s="1"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E95" s="1"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E96" s="1"/>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C97" s="1"/>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="F101" s="2"/>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F105" s="2"/>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E106" s="1"/>
       <c r="F106" s="2"/>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F108" s="2"/>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F109" s="2"/>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F110" s="2"/>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F111" s="2"/>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F112" s="2"/>
     </row>
-    <row r="113" spans="6:6">
+    <row r="113" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F113" s="2"/>
     </row>
-    <row r="114" spans="6:6">
+    <row r="114" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="6:6">
+    <row r="115" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F115" s="2"/>
     </row>
-    <row r="116" spans="6:6">
+    <row r="116" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="6:6">
+    <row r="117" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="6:6">
+    <row r="118" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F118" s="1"/>
     </row>
-    <row r="128" spans="6:6">
+    <row r="128" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F128" s="1"/>
     </row>
   </sheetData>
@@ -2139,21 +2154,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2170,7 +2185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2198,16 +2213,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2221,24 +2236,24 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
         <v>88</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>89</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>90</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" t="s">
-        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -2256,15 +2271,15 @@
         <v>2010</v>
       </c>
       <c r="H2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -2282,15 +2297,15 @@
         <v>2020</v>
       </c>
       <c r="H3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -2308,7 +2323,33 @@
         <v>2020</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5">
+        <v>2007</v>
+      </c>
+      <c r="D5">
+        <v>2010</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>2007</v>
+      </c>
+      <c r="G5">
+        <v>2010</v>
+      </c>
+      <c r="H5" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>